<commit_message>
DEMO FOR HOS VER
</commit_message>
<xml_diff>
--- a/reports/藥物辨識成功率總表.xlsx
+++ b/reports/藥物辨識成功率總表.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CC419"/>
+  <dimension ref="A1:CD419"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -834,6 +834,11 @@
           <t>2025-09-14_v6</t>
         </is>
       </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1061,6 +1066,9 @@
       <c r="CC2" t="n">
         <v>0.4</v>
       </c>
+      <c r="CD2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1284,6 +1292,9 @@
       <c r="CC3" t="n">
         <v>1</v>
       </c>
+      <c r="CD3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1505,6 +1516,9 @@
       <c r="CC4" t="n">
         <v>0.1428571428571428</v>
       </c>
+      <c r="CD4" t="n">
+        <v>0.1428571428571428</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1726,6 +1740,9 @@
       <c r="CC5" t="n">
         <v>1</v>
       </c>
+      <c r="CD5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1947,6 +1964,9 @@
       <c r="CC6" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD6" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2168,6 +2188,9 @@
       <c r="CC7" t="n">
         <v>0.4444444444444444</v>
       </c>
+      <c r="CD7" t="n">
+        <v>0.5555555555555556</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -2389,6 +2412,9 @@
       <c r="CC8" t="n">
         <v>0.1111111111111111</v>
       </c>
+      <c r="CD8" t="n">
+        <v>0.3333333333333333</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -2610,6 +2636,9 @@
       <c r="CC9" t="n">
         <v>0.6666666666666666</v>
       </c>
+      <c r="CD9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -2831,6 +2860,9 @@
       <c r="CC10" t="n">
         <v>0.6</v>
       </c>
+      <c r="CD10" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -3050,6 +3082,9 @@
         <v>1</v>
       </c>
       <c r="CC11" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3215,6 +3250,9 @@
       <c r="CC12" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD12" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -3436,6 +3474,9 @@
       <c r="CC13" t="n">
         <v>0</v>
       </c>
+      <c r="CD13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -3657,6 +3698,9 @@
       <c r="CC14" t="n">
         <v>0</v>
       </c>
+      <c r="CD14" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -3878,6 +3922,9 @@
       <c r="CC15" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD15" t="n">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -4099,6 +4146,9 @@
       <c r="CC16" t="n">
         <v>1</v>
       </c>
+      <c r="CD16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -4320,6 +4370,9 @@
       <c r="CC17" t="n">
         <v>0</v>
       </c>
+      <c r="CD17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -4541,6 +4594,9 @@
       <c r="CC18" t="n">
         <v>1</v>
       </c>
+      <c r="CD18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -4762,6 +4818,9 @@
       <c r="CC19" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD19" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -4983,6 +5042,9 @@
       <c r="CC20" t="n">
         <v>0</v>
       </c>
+      <c r="CD20" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -5204,6 +5266,9 @@
       <c r="CC21" t="n">
         <v>1</v>
       </c>
+      <c r="CD21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -5425,6 +5490,9 @@
       <c r="CC22" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD22" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -5646,6 +5714,9 @@
       <c r="CC23" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD23" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -5867,6 +5938,9 @@
       <c r="CC24" t="n">
         <v>0.2</v>
       </c>
+      <c r="CD24" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -6088,6 +6162,9 @@
       <c r="CC25" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD25" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -6309,6 +6386,9 @@
       <c r="CC26" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD26" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -6530,6 +6610,9 @@
       <c r="CC27" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD27" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -6751,6 +6834,9 @@
       <c r="CC28" t="n">
         <v>0.5555555555555556</v>
       </c>
+      <c r="CD28" t="n">
+        <v>0.5555555555555556</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -6972,6 +7058,9 @@
       <c r="CC29" t="n">
         <v>1</v>
       </c>
+      <c r="CD29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -7193,6 +7282,9 @@
       <c r="CC30" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD30" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -7414,6 +7506,9 @@
       <c r="CC31" t="n">
         <v>0</v>
       </c>
+      <c r="CD31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -7635,6 +7730,9 @@
       <c r="CC32" t="n">
         <v>0</v>
       </c>
+      <c r="CD32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -7856,6 +7954,9 @@
       <c r="CC33" t="n">
         <v>0</v>
       </c>
+      <c r="CD33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -8077,6 +8178,9 @@
       <c r="CC34" t="n">
         <v>1</v>
       </c>
+      <c r="CD34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -8298,6 +8402,9 @@
       <c r="CC35" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD35" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -8519,6 +8626,9 @@
       <c r="CC36" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD36" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -8740,6 +8850,9 @@
       <c r="CC37" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD37" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -8961,6 +9074,9 @@
       <c r="CC38" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD38" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -9182,6 +9298,9 @@
       <c r="CC39" t="n">
         <v>1</v>
       </c>
+      <c r="CD39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -9401,6 +9520,9 @@
         <v>1</v>
       </c>
       <c r="CC40" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD40" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9566,6 +9688,9 @@
       <c r="CC41" t="n">
         <v>0</v>
       </c>
+      <c r="CD41" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -9787,6 +9912,9 @@
       <c r="CC42" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD42" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -10008,6 +10136,9 @@
       <c r="CC43" t="n">
         <v>1</v>
       </c>
+      <c r="CD43" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -10229,6 +10360,9 @@
       <c r="CC44" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD44" t="n">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -10450,6 +10584,9 @@
       <c r="CC45" t="n">
         <v>0</v>
       </c>
+      <c r="CD45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -10671,6 +10808,9 @@
       <c r="CC46" t="n">
         <v>1</v>
       </c>
+      <c r="CD46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -10892,6 +11032,9 @@
       <c r="CC47" t="n">
         <v>0</v>
       </c>
+      <c r="CD47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -11113,6 +11256,9 @@
       <c r="CC48" t="n">
         <v>0</v>
       </c>
+      <c r="CD48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -11334,6 +11480,9 @@
       <c r="CC49" t="n">
         <v>0</v>
       </c>
+      <c r="CD49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -11555,6 +11704,9 @@
       <c r="CC50" t="n">
         <v>0</v>
       </c>
+      <c r="CD50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -11776,6 +11928,9 @@
       <c r="CC51" t="n">
         <v>1</v>
       </c>
+      <c r="CD51" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -11997,6 +12152,9 @@
       <c r="CC52" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD52" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -12218,6 +12376,9 @@
       <c r="CC53" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD53" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -12439,6 +12600,9 @@
       <c r="CC54" t="n">
         <v>0</v>
       </c>
+      <c r="CD54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -12660,6 +12824,9 @@
       <c r="CC55" t="n">
         <v>0</v>
       </c>
+      <c r="CD55" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -12881,6 +13048,9 @@
       <c r="CC56" t="n">
         <v>0</v>
       </c>
+      <c r="CD56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -13102,6 +13272,9 @@
       <c r="CC57" t="n">
         <v>0</v>
       </c>
+      <c r="CD57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -13323,6 +13496,9 @@
       <c r="CC58" t="n">
         <v>0</v>
       </c>
+      <c r="CD58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -13544,6 +13720,9 @@
       <c r="CC59" t="n">
         <v>0</v>
       </c>
+      <c r="CD59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -13765,6 +13944,9 @@
       <c r="CC60" t="n">
         <v>1</v>
       </c>
+      <c r="CD60" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
@@ -13986,6 +14168,9 @@
       <c r="CC61" t="n">
         <v>0</v>
       </c>
+      <c r="CD61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
@@ -14207,6 +14392,9 @@
       <c r="CC62" t="n">
         <v>0</v>
       </c>
+      <c r="CD62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -14428,6 +14616,9 @@
       <c r="CC63" t="n">
         <v>0.3333333333333333</v>
       </c>
+      <c r="CD63" t="n">
+        <v>0.6666666666666666</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -14649,6 +14840,9 @@
       <c r="CC64" t="n">
         <v>1</v>
       </c>
+      <c r="CD64" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -14870,6 +15064,9 @@
       <c r="CC65" t="n">
         <v>0.125</v>
       </c>
+      <c r="CD65" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -15091,6 +15288,9 @@
       <c r="CC66" t="n">
         <v>0</v>
       </c>
+      <c r="CD66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -15312,6 +15512,9 @@
       <c r="CC67" t="n">
         <v>0</v>
       </c>
+      <c r="CD67" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
@@ -15533,6 +15736,9 @@
       <c r="CC68" t="n">
         <v>0.125</v>
       </c>
+      <c r="CD68" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
@@ -15754,6 +15960,9 @@
       <c r="CC69" t="n">
         <v>0</v>
       </c>
+      <c r="CD69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -15975,6 +16184,9 @@
       <c r="CC70" t="n">
         <v>0.1666666666666667</v>
       </c>
+      <c r="CD70" t="n">
+        <v>0.3333333333333333</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -16196,6 +16408,9 @@
       <c r="CC71" t="n">
         <v>0</v>
       </c>
+      <c r="CD71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -16417,6 +16632,9 @@
       <c r="CC72" t="n">
         <v>0</v>
       </c>
+      <c r="CD72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
@@ -16638,6 +16856,9 @@
       <c r="CC73" t="n">
         <v>0</v>
       </c>
+      <c r="CD73" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
@@ -16859,6 +17080,9 @@
       <c r="CC74" t="n">
         <v>0</v>
       </c>
+      <c r="CD74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
@@ -17080,6 +17304,9 @@
       <c r="CC75" t="n">
         <v>0</v>
       </c>
+      <c r="CD75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
@@ -17301,6 +17528,9 @@
       <c r="CC76" t="n">
         <v>0</v>
       </c>
+      <c r="CD76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
@@ -17522,6 +17752,9 @@
       <c r="CC77" t="n">
         <v>1</v>
       </c>
+      <c r="CD77" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
@@ -17743,6 +17976,9 @@
       <c r="CC78" t="n">
         <v>0.125</v>
       </c>
+      <c r="CD78" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -17964,6 +18200,9 @@
       <c r="CC79" t="n">
         <v>1</v>
       </c>
+      <c r="CD79" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
@@ -18185,6 +18424,9 @@
       <c r="CC80" t="n">
         <v>0</v>
       </c>
+      <c r="CD80" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
@@ -18406,6 +18648,9 @@
       <c r="CC81" t="n">
         <v>0</v>
       </c>
+      <c r="CD81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
@@ -18627,6 +18872,9 @@
       <c r="CC82" t="n">
         <v>0.125</v>
       </c>
+      <c r="CD82" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
@@ -18848,6 +19096,9 @@
       <c r="CC83" t="n">
         <v>0</v>
       </c>
+      <c r="CD83" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
@@ -19069,6 +19320,9 @@
       <c r="CC84" t="n">
         <v>0.1111111111111111</v>
       </c>
+      <c r="CD84" t="n">
+        <v>0.1111111111111111</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
@@ -19290,6 +19544,9 @@
       <c r="CC85" t="n">
         <v>0</v>
       </c>
+      <c r="CD85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
@@ -19511,6 +19768,9 @@
       <c r="CC86" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD86" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
@@ -19732,6 +19992,9 @@
       <c r="CC87" t="n">
         <v>0</v>
       </c>
+      <c r="CD87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
@@ -19953,6 +20216,9 @@
       <c r="CC88" t="n">
         <v>0.125</v>
       </c>
+      <c r="CD88" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
@@ -20174,6 +20440,9 @@
       <c r="CC89" t="n">
         <v>0</v>
       </c>
+      <c r="CD89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
@@ -20395,6 +20664,9 @@
       <c r="CC90" t="n">
         <v>0</v>
       </c>
+      <c r="CD90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
@@ -20616,6 +20888,9 @@
       <c r="CC91" t="n">
         <v>0</v>
       </c>
+      <c r="CD91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
@@ -20837,6 +21112,9 @@
       <c r="CC92" t="n">
         <v>0</v>
       </c>
+      <c r="CD92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
@@ -21058,6 +21336,9 @@
       <c r="CC93" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD93" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
@@ -21279,6 +21560,9 @@
       <c r="CC94" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD94" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
@@ -21500,6 +21784,9 @@
       <c r="CC95" t="n">
         <v>1</v>
       </c>
+      <c r="CD95" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
@@ -21721,6 +22008,9 @@
       <c r="CC96" t="n">
         <v>0</v>
       </c>
+      <c r="CD96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
@@ -21942,6 +22232,9 @@
       <c r="CC97" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD97" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
@@ -22163,6 +22456,9 @@
       <c r="CC98" t="n">
         <v>1</v>
       </c>
+      <c r="CD98" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
@@ -22384,6 +22680,9 @@
       <c r="CC99" t="n">
         <v>0.125</v>
       </c>
+      <c r="CD99" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
@@ -22605,6 +22904,9 @@
       <c r="CC100" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD100" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
@@ -22826,6 +23128,9 @@
       <c r="CC101" t="n">
         <v>1</v>
       </c>
+      <c r="CD101" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
@@ -23047,6 +23352,9 @@
       <c r="CC102" t="n">
         <v>0</v>
       </c>
+      <c r="CD102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
@@ -23268,6 +23576,9 @@
       <c r="CC103" t="n">
         <v>0.375</v>
       </c>
+      <c r="CD103" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
@@ -23489,6 +23800,9 @@
       <c r="CC104" t="n">
         <v>1</v>
       </c>
+      <c r="CD104" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
@@ -23710,6 +24024,9 @@
       <c r="CC105" t="n">
         <v>0</v>
       </c>
+      <c r="CD105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
@@ -23931,6 +24248,9 @@
       <c r="CC106" t="n">
         <v>0</v>
       </c>
+      <c r="CD106" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
@@ -24152,6 +24472,9 @@
       <c r="CC107" t="n">
         <v>0</v>
       </c>
+      <c r="CD107" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
@@ -24373,6 +24696,9 @@
       <c r="CC108" t="n">
         <v>0</v>
       </c>
+      <c r="CD108" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
@@ -24594,6 +24920,9 @@
       <c r="CC109" t="n">
         <v>0.125</v>
       </c>
+      <c r="CD109" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
@@ -24815,6 +25144,9 @@
       <c r="CC110" t="n">
         <v>0</v>
       </c>
+      <c r="CD110" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
@@ -25036,6 +25368,9 @@
       <c r="CC111" t="n">
         <v>1</v>
       </c>
+      <c r="CD111" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
@@ -25257,6 +25592,9 @@
       <c r="CC112" t="n">
         <v>1</v>
       </c>
+      <c r="CD112" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
@@ -25478,6 +25816,9 @@
       <c r="CC113" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD113" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
@@ -25699,6 +26040,9 @@
       <c r="CC114" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD114" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
@@ -25920,6 +26264,9 @@
       <c r="CC115" t="n">
         <v>0</v>
       </c>
+      <c r="CD115" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
@@ -26141,6 +26488,9 @@
       <c r="CC116" t="n">
         <v>0</v>
       </c>
+      <c r="CD116" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
@@ -26362,6 +26712,9 @@
       <c r="CC117" t="n">
         <v>1</v>
       </c>
+      <c r="CD117" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
@@ -26583,6 +26936,9 @@
       <c r="CC118" t="n">
         <v>0</v>
       </c>
+      <c r="CD118" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
@@ -26804,6 +27160,9 @@
       <c r="CC119" t="n">
         <v>0.625</v>
       </c>
+      <c r="CD119" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
@@ -27025,6 +27384,9 @@
       <c r="CC120" t="n">
         <v>0.125</v>
       </c>
+      <c r="CD120" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
@@ -27246,6 +27608,9 @@
       <c r="CC121" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD121" t="n">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
@@ -27467,6 +27832,9 @@
       <c r="CC122" t="n">
         <v>0</v>
       </c>
+      <c r="CD122" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
@@ -27688,6 +28056,9 @@
       <c r="CC123" t="n">
         <v>0</v>
       </c>
+      <c r="CD123" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
@@ -27909,6 +28280,9 @@
       <c r="CC124" t="n">
         <v>0</v>
       </c>
+      <c r="CD124" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
@@ -28130,6 +28504,9 @@
       <c r="CC125" t="n">
         <v>0</v>
       </c>
+      <c r="CD125" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
@@ -28351,6 +28728,9 @@
       <c r="CC126" t="n">
         <v>0</v>
       </c>
+      <c r="CD126" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
@@ -28572,6 +28952,9 @@
       <c r="CC127" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD127" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
@@ -28793,6 +29176,9 @@
       <c r="CC128" t="n">
         <v>0</v>
       </c>
+      <c r="CD128" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
@@ -29014,6 +29400,9 @@
       <c r="CC129" t="n">
         <v>1</v>
       </c>
+      <c r="CD129" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
@@ -29235,6 +29624,9 @@
       <c r="CC130" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD130" t="n">
+        <v>0.875</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
@@ -29456,6 +29848,9 @@
       <c r="CC131" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD131" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
@@ -29677,6 +30072,9 @@
       <c r="CC132" t="n">
         <v>0</v>
       </c>
+      <c r="CD132" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
@@ -29898,6 +30296,9 @@
       <c r="CC133" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD133" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
@@ -30119,6 +30520,9 @@
       <c r="CC134" t="n">
         <v>0</v>
       </c>
+      <c r="CD134" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
@@ -30340,6 +30744,9 @@
       <c r="CC135" t="n">
         <v>0</v>
       </c>
+      <c r="CD135" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
@@ -30561,6 +30968,9 @@
       <c r="CC136" t="n">
         <v>0</v>
       </c>
+      <c r="CD136" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
@@ -30782,6 +31192,9 @@
       <c r="CC137" t="n">
         <v>0.125</v>
       </c>
+      <c r="CD137" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
@@ -31003,6 +31416,9 @@
       <c r="CC138" t="n">
         <v>0</v>
       </c>
+      <c r="CD138" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
@@ -31224,6 +31640,9 @@
       <c r="CC139" t="n">
         <v>0</v>
       </c>
+      <c r="CD139" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
@@ -31445,6 +31864,9 @@
       <c r="CC140" t="n">
         <v>0.125</v>
       </c>
+      <c r="CD140" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
@@ -31666,6 +32088,9 @@
       <c r="CC141" t="n">
         <v>0.375</v>
       </c>
+      <c r="CD141" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
@@ -31887,6 +32312,9 @@
       <c r="CC142" t="n">
         <v>0</v>
       </c>
+      <c r="CD142" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
@@ -32108,6 +32536,9 @@
       <c r="CC143" t="n">
         <v>0</v>
       </c>
+      <c r="CD143" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
@@ -32329,6 +32760,9 @@
       <c r="CC144" t="n">
         <v>1</v>
       </c>
+      <c r="CD144" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
@@ -32550,6 +32984,9 @@
       <c r="CC145" t="n">
         <v>0</v>
       </c>
+      <c r="CD145" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
@@ -32771,6 +33208,9 @@
       <c r="CC146" t="n">
         <v>0</v>
       </c>
+      <c r="CD146" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
@@ -32992,6 +33432,9 @@
       <c r="CC147" t="n">
         <v>0</v>
       </c>
+      <c r="CD147" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
@@ -33213,6 +33656,9 @@
       <c r="CC148" t="n">
         <v>0</v>
       </c>
+      <c r="CD148" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
@@ -33434,6 +33880,9 @@
       <c r="CC149" t="n">
         <v>1</v>
       </c>
+      <c r="CD149" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="inlineStr">
@@ -33655,6 +34104,9 @@
       <c r="CC150" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD150" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="inlineStr">
@@ -33876,6 +34328,9 @@
       <c r="CC151" t="n">
         <v>0</v>
       </c>
+      <c r="CD151" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
@@ -34097,6 +34552,9 @@
       <c r="CC152" t="n">
         <v>0</v>
       </c>
+      <c r="CD152" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
@@ -34318,6 +34776,9 @@
       <c r="CC153" t="n">
         <v>1</v>
       </c>
+      <c r="CD153" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
@@ -34539,6 +35000,9 @@
       <c r="CC154" t="n">
         <v>0</v>
       </c>
+      <c r="CD154" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="inlineStr">
@@ -34760,6 +35224,9 @@
       <c r="CC155" t="n">
         <v>0.375</v>
       </c>
+      <c r="CD155" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="inlineStr">
@@ -34981,6 +35448,9 @@
       <c r="CC156" t="n">
         <v>0.125</v>
       </c>
+      <c r="CD156" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
@@ -35202,6 +35672,9 @@
       <c r="CC157" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD157" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
@@ -35423,6 +35896,9 @@
       <c r="CC158" t="n">
         <v>1</v>
       </c>
+      <c r="CD158" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
@@ -35644,6 +36120,9 @@
       <c r="CC159" t="n">
         <v>1</v>
       </c>
+      <c r="CD159" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
@@ -35865,6 +36344,9 @@
       <c r="CC160" t="n">
         <v>1</v>
       </c>
+      <c r="CD160" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
@@ -36086,6 +36568,9 @@
       <c r="CC161" t="n">
         <v>0</v>
       </c>
+      <c r="CD161" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
@@ -36307,6 +36792,9 @@
       <c r="CC162" t="n">
         <v>0</v>
       </c>
+      <c r="CD162" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
@@ -36528,6 +37016,9 @@
       <c r="CC163" t="n">
         <v>1</v>
       </c>
+      <c r="CD163" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
@@ -36749,6 +37240,9 @@
       <c r="CC164" t="n">
         <v>1</v>
       </c>
+      <c r="CD164" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
@@ -36970,6 +37464,9 @@
       <c r="CC165" t="n">
         <v>0</v>
       </c>
+      <c r="CD165" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
@@ -37191,6 +37688,9 @@
       <c r="CC166" t="n">
         <v>1</v>
       </c>
+      <c r="CD166" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
@@ -37412,6 +37912,9 @@
       <c r="CC167" t="n">
         <v>0</v>
       </c>
+      <c r="CD167" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
@@ -37633,6 +38136,9 @@
       <c r="CC168" t="n">
         <v>1</v>
       </c>
+      <c r="CD168" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
@@ -37854,6 +38360,9 @@
       <c r="CC169" t="n">
         <v>1</v>
       </c>
+      <c r="CD169" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
@@ -38075,6 +38584,9 @@
       <c r="CC170" t="n">
         <v>1</v>
       </c>
+      <c r="CD170" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
@@ -38296,6 +38808,9 @@
       <c r="CC171" t="n">
         <v>1</v>
       </c>
+      <c r="CD171" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
@@ -38517,6 +39032,9 @@
       <c r="CC172" t="n">
         <v>0.625</v>
       </c>
+      <c r="CD172" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
@@ -38738,6 +39256,9 @@
       <c r="CC173" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD173" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
@@ -38959,6 +39480,9 @@
       <c r="CC174" t="n">
         <v>1</v>
       </c>
+      <c r="CD174" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
@@ -39180,6 +39704,9 @@
       <c r="CC175" t="n">
         <v>0.8333333333333334</v>
       </c>
+      <c r="CD175" t="n">
+        <v>0.8333333333333334</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
@@ -39401,6 +39928,9 @@
       <c r="CC176" t="n">
         <v>0</v>
       </c>
+      <c r="CD176" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
@@ -39622,6 +40152,9 @@
       <c r="CC177" t="n">
         <v>0.3333333333333333</v>
       </c>
+      <c r="CD177" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
@@ -39843,6 +40376,9 @@
       <c r="CC178" t="n">
         <v>0</v>
       </c>
+      <c r="CD178" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
@@ -40064,6 +40600,9 @@
       <c r="CC179" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD179" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="inlineStr">
@@ -40285,6 +40824,9 @@
       <c r="CC180" t="n">
         <v>0.8</v>
       </c>
+      <c r="CD180" t="n">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="inlineStr">
@@ -40506,6 +41048,9 @@
       <c r="CC181" t="n">
         <v>0</v>
       </c>
+      <c r="CD181" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="inlineStr">
@@ -40727,6 +41272,9 @@
       <c r="CC182" t="n">
         <v>0</v>
       </c>
+      <c r="CD182" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="inlineStr">
@@ -40948,6 +41496,9 @@
       <c r="CC183" t="n">
         <v>1</v>
       </c>
+      <c r="CD183" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="inlineStr">
@@ -41169,6 +41720,9 @@
       <c r="CC184" t="n">
         <v>0.2857142857142857</v>
       </c>
+      <c r="CD184" t="n">
+        <v>0.5714285714285714</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="inlineStr">
@@ -41390,6 +41944,9 @@
       <c r="CC185" t="n">
         <v>0</v>
       </c>
+      <c r="CD185" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="inlineStr">
@@ -41611,6 +42168,9 @@
       <c r="CC186" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD186" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="inlineStr">
@@ -41832,6 +42392,9 @@
       <c r="CC187" t="n">
         <v>0.3333333333333333</v>
       </c>
+      <c r="CD187" t="n">
+        <v>0.6666666666666666</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="inlineStr">
@@ -42053,6 +42616,9 @@
       <c r="CC188" t="n">
         <v>0</v>
       </c>
+      <c r="CD188" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="inlineStr">
@@ -42274,6 +42840,9 @@
       <c r="CC189" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD189" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="inlineStr">
@@ -42495,6 +43064,9 @@
       <c r="CC190" t="n">
         <v>0.8</v>
       </c>
+      <c r="CD190" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="inlineStr">
@@ -42716,6 +43288,9 @@
       <c r="CC191" t="n">
         <v>1</v>
       </c>
+      <c r="CD191" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="inlineStr">
@@ -42937,6 +43512,9 @@
       <c r="CC192" t="n">
         <v>0</v>
       </c>
+      <c r="CD192" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="inlineStr">
@@ -43158,6 +43736,9 @@
       <c r="CC193" t="n">
         <v>1</v>
       </c>
+      <c r="CD193" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="inlineStr">
@@ -43379,6 +43960,9 @@
       <c r="CC194" t="n">
         <v>0</v>
       </c>
+      <c r="CD194" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="inlineStr">
@@ -43600,6 +44184,9 @@
       <c r="CC195" t="n">
         <v>1</v>
       </c>
+      <c r="CD195" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="inlineStr">
@@ -43821,6 +44408,9 @@
       <c r="CC196" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD196" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="inlineStr">
@@ -44042,6 +44632,9 @@
       <c r="CC197" t="n">
         <v>1</v>
       </c>
+      <c r="CD197" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="inlineStr">
@@ -44263,6 +44856,9 @@
       <c r="CC198" t="n">
         <v>0</v>
       </c>
+      <c r="CD198" t="n">
+        <v>0.1428571428571428</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="inlineStr">
@@ -44484,6 +45080,9 @@
       <c r="CC199" t="n">
         <v>0</v>
       </c>
+      <c r="CD199" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="inlineStr">
@@ -44705,6 +45304,9 @@
       <c r="CC200" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD200" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="inlineStr">
@@ -44926,6 +45528,9 @@
       <c r="CC201" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD201" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="inlineStr">
@@ -45147,6 +45752,9 @@
       <c r="CC202" t="n">
         <v>0.8</v>
       </c>
+      <c r="CD202" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="inlineStr">
@@ -45368,6 +45976,9 @@
       <c r="CC203" t="n">
         <v>0</v>
       </c>
+      <c r="CD203" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="inlineStr">
@@ -45589,6 +46200,9 @@
       <c r="CC204" t="n">
         <v>0</v>
       </c>
+      <c r="CD204" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="inlineStr">
@@ -45809,6 +46423,9 @@
       </c>
       <c r="CC205" t="n">
         <v>0.1666666666666667</v>
+      </c>
+      <c r="CD205" t="n">
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="206">
@@ -45961,6 +46578,9 @@
       <c r="CC206" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD206" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="inlineStr">
@@ -46182,6 +46802,9 @@
       <c r="CC207" t="n">
         <v>0.4</v>
       </c>
+      <c r="CD207" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="inlineStr">
@@ -46403,6 +47026,9 @@
       <c r="CC208" t="n">
         <v>1</v>
       </c>
+      <c r="CD208" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="inlineStr">
@@ -46624,6 +47250,9 @@
       <c r="CC209" t="n">
         <v>0</v>
       </c>
+      <c r="CD209" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="inlineStr">
@@ -46845,6 +47474,9 @@
       <c r="CC210" t="n">
         <v>0</v>
       </c>
+      <c r="CD210" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="inlineStr">
@@ -47066,6 +47698,9 @@
       <c r="CC211" t="n">
         <v>0.375</v>
       </c>
+      <c r="CD211" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="inlineStr">
@@ -47287,6 +47922,9 @@
       <c r="CC212" t="n">
         <v>0.1818181818181818</v>
       </c>
+      <c r="CD212" t="n">
+        <v>0.3636363636363636</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="inlineStr">
@@ -47508,6 +48146,9 @@
       <c r="CC213" t="n">
         <v>0</v>
       </c>
+      <c r="CD213" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="inlineStr">
@@ -47729,6 +48370,9 @@
       <c r="CC214" t="n">
         <v>0</v>
       </c>
+      <c r="CD214" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="inlineStr">
@@ -47950,6 +48594,9 @@
       <c r="CC215" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD215" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="inlineStr">
@@ -48171,6 +48818,9 @@
       <c r="CC216" t="n">
         <v>0</v>
       </c>
+      <c r="CD216" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="inlineStr">
@@ -48392,6 +49042,9 @@
       <c r="CC217" t="n">
         <v>1</v>
       </c>
+      <c r="CD217" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
@@ -48613,6 +49266,9 @@
       <c r="CC218" t="n">
         <v>1</v>
       </c>
+      <c r="CD218" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
@@ -48834,6 +49490,9 @@
       <c r="CC219" t="n">
         <v>1</v>
       </c>
+      <c r="CD219" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
@@ -49055,6 +49714,9 @@
       <c r="CC220" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD220" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
@@ -49276,6 +49938,9 @@
       <c r="CC221" t="n">
         <v>0</v>
       </c>
+      <c r="CD221" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
@@ -49497,6 +50162,9 @@
       <c r="CC222" t="n">
         <v>0</v>
       </c>
+      <c r="CD222" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
@@ -49718,6 +50386,9 @@
       <c r="CC223" t="n">
         <v>0.8</v>
       </c>
+      <c r="CD223" t="n">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
@@ -49939,6 +50610,9 @@
       <c r="CC224" t="n">
         <v>0</v>
       </c>
+      <c r="CD224" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
@@ -50160,6 +50834,9 @@
       <c r="CC225" t="n">
         <v>0</v>
       </c>
+      <c r="CD225" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
@@ -50381,6 +51058,9 @@
       <c r="CC226" t="n">
         <v>0</v>
       </c>
+      <c r="CD226" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
@@ -50602,6 +51282,9 @@
       <c r="CC227" t="n">
         <v>1</v>
       </c>
+      <c r="CD227" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
@@ -50823,6 +51506,9 @@
       <c r="CC228" t="n">
         <v>0</v>
       </c>
+      <c r="CD228" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
@@ -51044,6 +51730,9 @@
       <c r="CC229" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD229" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
@@ -51265,6 +51954,9 @@
       <c r="CC230" t="n">
         <v>1</v>
       </c>
+      <c r="CD230" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
@@ -51486,6 +52178,9 @@
       <c r="CC231" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD231" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
@@ -51707,6 +52402,9 @@
       <c r="CC232" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD232" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
@@ -51928,6 +52626,9 @@
       <c r="CC233" t="n">
         <v>0</v>
       </c>
+      <c r="CD233" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
@@ -52149,6 +52850,9 @@
       <c r="CC234" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD234" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
@@ -52370,6 +53074,9 @@
       <c r="CC235" t="n">
         <v>1</v>
       </c>
+      <c r="CD235" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
@@ -52591,6 +53298,9 @@
       <c r="CC236" t="n">
         <v>0</v>
       </c>
+      <c r="CD236" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
@@ -52812,6 +53522,9 @@
       <c r="CC237" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD237" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
@@ -53033,6 +53746,9 @@
       <c r="CC238" t="n">
         <v>0</v>
       </c>
+      <c r="CD238" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
@@ -53254,6 +53970,9 @@
       <c r="CC239" t="n">
         <v>0</v>
       </c>
+      <c r="CD239" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
@@ -53475,6 +54194,9 @@
       <c r="CC240" t="n">
         <v>1</v>
       </c>
+      <c r="CD240" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
@@ -53696,6 +54418,9 @@
       <c r="CC241" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD241" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
@@ -53917,6 +54642,9 @@
       <c r="CC242" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD242" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
@@ -54138,6 +54866,9 @@
       <c r="CC243" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD243" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
@@ -54359,6 +55090,9 @@
       <c r="CC244" t="n">
         <v>1</v>
       </c>
+      <c r="CD244" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
@@ -54580,6 +55314,9 @@
       <c r="CC245" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD245" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
@@ -54801,6 +55538,9 @@
       <c r="CC246" t="n">
         <v>0</v>
       </c>
+      <c r="CD246" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
@@ -55022,6 +55762,9 @@
       <c r="CC247" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD247" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
@@ -55243,6 +55986,9 @@
       <c r="CC248" t="n">
         <v>0.4</v>
       </c>
+      <c r="CD248" t="n">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
@@ -55464,6 +56210,9 @@
       <c r="CC249" t="n">
         <v>0</v>
       </c>
+      <c r="CD249" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
@@ -55685,6 +56434,9 @@
       <c r="CC250" t="n">
         <v>0</v>
       </c>
+      <c r="CD250" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
@@ -55906,6 +56658,9 @@
       <c r="CC251" t="n">
         <v>0.375</v>
       </c>
+      <c r="CD251" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
@@ -56127,6 +56882,9 @@
       <c r="CC252" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD252" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
@@ -56348,6 +57106,9 @@
       <c r="CC253" t="n">
         <v>0</v>
       </c>
+      <c r="CD253" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
@@ -56569,6 +57330,9 @@
       <c r="CC254" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD254" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
@@ -56790,6 +57554,9 @@
       <c r="CC255" t="n">
         <v>1</v>
       </c>
+      <c r="CD255" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
@@ -57011,6 +57778,9 @@
       <c r="CC256" t="n">
         <v>0</v>
       </c>
+      <c r="CD256" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
@@ -57232,6 +58002,9 @@
       <c r="CC257" t="n">
         <v>1</v>
       </c>
+      <c r="CD257" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
@@ -57453,6 +58226,9 @@
       <c r="CC258" t="n">
         <v>0.6</v>
       </c>
+      <c r="CD258" t="n">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
@@ -57674,6 +58450,9 @@
       <c r="CC259" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD259" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
@@ -57895,6 +58674,9 @@
       <c r="CC260" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD260" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
@@ -58116,6 +58898,9 @@
       <c r="CC261" t="n">
         <v>1</v>
       </c>
+      <c r="CD261" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
@@ -58337,6 +59122,9 @@
       <c r="CC262" t="n">
         <v>0</v>
       </c>
+      <c r="CD262" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
@@ -58558,6 +59346,9 @@
       <c r="CC263" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD263" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
@@ -58779,6 +59570,9 @@
       <c r="CC264" t="n">
         <v>1</v>
       </c>
+      <c r="CD264" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
@@ -59000,6 +59794,9 @@
       <c r="CC265" t="n">
         <v>0</v>
       </c>
+      <c r="CD265" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
@@ -59221,6 +60018,9 @@
       <c r="CC266" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD266" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
@@ -59442,6 +60242,9 @@
       <c r="CC267" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD267" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
@@ -59663,6 +60466,9 @@
       <c r="CC268" t="n">
         <v>0</v>
       </c>
+      <c r="CD268" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
@@ -59884,6 +60690,9 @@
       <c r="CC269" t="n">
         <v>0</v>
       </c>
+      <c r="CD269" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
@@ -60103,6 +60912,9 @@
         <v>0.7142857142857143</v>
       </c>
       <c r="CC270" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="CD270" t="n">
         <v>0.7142857142857143</v>
       </c>
     </row>
@@ -60202,6 +61014,7 @@
       <c r="CA271" t="inlineStr"/>
       <c r="CB271" t="inlineStr"/>
       <c r="CC271" t="inlineStr"/>
+      <c r="CD271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
@@ -60423,6 +61236,9 @@
       <c r="CC272" t="n">
         <v>1</v>
       </c>
+      <c r="CD272" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
@@ -60644,6 +61460,9 @@
       <c r="CC273" t="n">
         <v>0.1666666666666667</v>
       </c>
+      <c r="CD273" t="n">
+        <v>0.1666666666666667</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
@@ -60865,6 +61684,9 @@
       <c r="CC274" t="n">
         <v>0</v>
       </c>
+      <c r="CD274" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
@@ -61086,6 +61908,9 @@
       <c r="CC275" t="n">
         <v>1</v>
       </c>
+      <c r="CD275" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
@@ -61307,6 +62132,9 @@
       <c r="CC276" t="n">
         <v>0</v>
       </c>
+      <c r="CD276" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
@@ -61528,6 +62356,9 @@
       <c r="CC277" t="n">
         <v>0.6666666666666666</v>
       </c>
+      <c r="CD277" t="n">
+        <v>0.6666666666666666</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
@@ -61749,6 +62580,9 @@
       <c r="CC278" t="n">
         <v>0.4285714285714285</v>
       </c>
+      <c r="CD278" t="n">
+        <v>0.5714285714285714</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
@@ -61970,6 +62804,9 @@
       <c r="CC279" t="n">
         <v>0.1428571428571428</v>
       </c>
+      <c r="CD279" t="n">
+        <v>0.2857142857142857</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
@@ -62191,6 +63028,9 @@
       <c r="CC280" t="n">
         <v>0</v>
       </c>
+      <c r="CD280" t="n">
+        <v>0.4285714285714285</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
@@ -62412,6 +63252,9 @@
       <c r="CC281" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD281" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
@@ -62633,6 +63476,9 @@
       <c r="CC282" t="n">
         <v>0.4285714285714285</v>
       </c>
+      <c r="CD282" t="n">
+        <v>0.7142857142857143</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
@@ -62854,6 +63700,9 @@
       <c r="CC283" t="n">
         <v>0.625</v>
       </c>
+      <c r="CD283" t="n">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
@@ -63075,6 +63924,9 @@
       <c r="CC284" t="n">
         <v>1</v>
       </c>
+      <c r="CD284" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
@@ -63296,6 +64148,9 @@
       <c r="CC285" t="n">
         <v>0.7777777777777778</v>
       </c>
+      <c r="CD285" t="n">
+        <v>0.7777777777777778</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
@@ -63517,6 +64372,9 @@
       <c r="CC286" t="n">
         <v>0.8</v>
       </c>
+      <c r="CD286" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
@@ -63738,6 +64596,9 @@
       <c r="CC287" t="n">
         <v>0</v>
       </c>
+      <c r="CD287" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
@@ -63959,6 +64820,9 @@
       <c r="CC288" t="n">
         <v>1</v>
       </c>
+      <c r="CD288" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
@@ -64180,6 +65044,9 @@
       <c r="CC289" t="n">
         <v>0</v>
       </c>
+      <c r="CD289" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
@@ -64401,6 +65268,9 @@
       <c r="CC290" t="n">
         <v>0</v>
       </c>
+      <c r="CD290" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
@@ -64622,6 +65492,9 @@
       <c r="CC291" t="n">
         <v>1</v>
       </c>
+      <c r="CD291" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
@@ -64843,6 +65716,9 @@
       <c r="CC292" t="n">
         <v>0</v>
       </c>
+      <c r="CD292" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
@@ -65064,6 +65940,9 @@
       <c r="CC293" t="n">
         <v>0.3333333333333333</v>
       </c>
+      <c r="CD293" t="n">
+        <v>0.6666666666666666</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
@@ -65285,6 +66164,9 @@
       <c r="CC294" t="n">
         <v>0</v>
       </c>
+      <c r="CD294" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
@@ -65506,6 +66388,9 @@
       <c r="CC295" t="n">
         <v>0.7142857142857143</v>
       </c>
+      <c r="CD295" t="n">
+        <v>0.7142857142857143</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
@@ -65727,6 +66612,9 @@
       <c r="CC296" t="n">
         <v>0.375</v>
       </c>
+      <c r="CD296" t="n">
+        <v>0.375</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
@@ -65948,6 +66836,9 @@
       <c r="CC297" t="n">
         <v>0.8333333333333334</v>
       </c>
+      <c r="CD297" t="n">
+        <v>0.8333333333333334</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
@@ -66169,6 +67060,9 @@
       <c r="CC298" t="n">
         <v>0.1666666666666667</v>
       </c>
+      <c r="CD298" t="n">
+        <v>0.1666666666666667</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
@@ -66390,6 +67284,9 @@
       <c r="CC299" t="n">
         <v>0.1666666666666667</v>
       </c>
+      <c r="CD299" t="n">
+        <v>0.1666666666666667</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
@@ -66611,6 +67508,9 @@
       <c r="CC300" t="n">
         <v>0</v>
       </c>
+      <c r="CD300" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
@@ -66832,6 +67732,9 @@
       <c r="CC301" t="n">
         <v>1</v>
       </c>
+      <c r="CD301" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
@@ -67053,6 +67956,9 @@
       <c r="CC302" t="n">
         <v>0</v>
       </c>
+      <c r="CD302" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
@@ -67274,6 +68180,9 @@
       <c r="CC303" t="n">
         <v>1</v>
       </c>
+      <c r="CD303" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
@@ -67495,6 +68404,9 @@
       <c r="CC304" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD304" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
@@ -67716,6 +68628,9 @@
       <c r="CC305" t="n">
         <v>0</v>
       </c>
+      <c r="CD305" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
@@ -67937,6 +68852,9 @@
       <c r="CC306" t="n">
         <v>0.3333333333333333</v>
       </c>
+      <c r="CD306" t="n">
+        <v>0.6666666666666666</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
@@ -68158,6 +69076,9 @@
       <c r="CC307" t="n">
         <v>0</v>
       </c>
+      <c r="CD307" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
@@ -68379,6 +69300,9 @@
       <c r="CC308" t="n">
         <v>0</v>
       </c>
+      <c r="CD308" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
@@ -68600,6 +69524,9 @@
       <c r="CC309" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD309" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
@@ -68821,6 +69748,9 @@
       <c r="CC310" t="n">
         <v>0</v>
       </c>
+      <c r="CD310" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
@@ -69042,6 +69972,9 @@
       <c r="CC311" t="n">
         <v>0</v>
       </c>
+      <c r="CD311" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
@@ -69263,6 +70196,9 @@
       <c r="CC312" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD312" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
@@ -69484,6 +70420,9 @@
       <c r="CC313" t="n">
         <v>1</v>
       </c>
+      <c r="CD313" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
@@ -69705,6 +70644,9 @@
       <c r="CC314" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD314" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
@@ -69926,6 +70868,9 @@
       <c r="CC315" t="n">
         <v>0</v>
       </c>
+      <c r="CD315" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
@@ -70147,6 +71092,9 @@
       <c r="CC316" t="n">
         <v>0.6</v>
       </c>
+      <c r="CD316" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
@@ -70368,6 +71316,9 @@
       <c r="CC317" t="n">
         <v>0</v>
       </c>
+      <c r="CD317" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
@@ -70589,6 +71540,9 @@
       <c r="CC318" t="n">
         <v>0</v>
       </c>
+      <c r="CD318" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
@@ -70810,6 +71764,9 @@
       <c r="CC319" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD319" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
@@ -71031,6 +71988,9 @@
       <c r="CC320" t="n">
         <v>1</v>
       </c>
+      <c r="CD320" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
@@ -71252,6 +72212,9 @@
       <c r="CC321" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD321" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
@@ -71473,6 +72436,9 @@
       <c r="CC322" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD322" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
@@ -71694,6 +72660,9 @@
       <c r="CC323" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD323" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
@@ -71915,6 +72884,9 @@
       <c r="CC324" t="n">
         <v>0</v>
       </c>
+      <c r="CD324" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
@@ -72136,6 +73108,9 @@
       <c r="CC325" t="n">
         <v>1</v>
       </c>
+      <c r="CD325" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
@@ -72357,6 +73332,9 @@
       <c r="CC326" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD326" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
@@ -72578,6 +73556,9 @@
       <c r="CC327" t="n">
         <v>0</v>
       </c>
+      <c r="CD327" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
@@ -72799,6 +73780,9 @@
       <c r="CC328" t="n">
         <v>1</v>
       </c>
+      <c r="CD328" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
@@ -73020,6 +74004,9 @@
       <c r="CC329" t="n">
         <v>1</v>
       </c>
+      <c r="CD329" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
@@ -73241,6 +74228,9 @@
       <c r="CC330" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD330" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="inlineStr">
@@ -73462,6 +74452,9 @@
       <c r="CC331" t="n">
         <v>1</v>
       </c>
+      <c r="CD331" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="inlineStr">
@@ -73683,6 +74676,9 @@
       <c r="CC332" t="n">
         <v>0</v>
       </c>
+      <c r="CD332" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="inlineStr">
@@ -73904,6 +74900,9 @@
       <c r="CC333" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD333" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="inlineStr">
@@ -74125,6 +75124,9 @@
       <c r="CC334" t="n">
         <v>1</v>
       </c>
+      <c r="CD334" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="inlineStr">
@@ -74346,6 +75348,9 @@
       <c r="CC335" t="n">
         <v>0</v>
       </c>
+      <c r="CD335" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="inlineStr">
@@ -74567,6 +75572,9 @@
       <c r="CC336" t="n">
         <v>1</v>
       </c>
+      <c r="CD336" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="inlineStr">
@@ -74788,6 +75796,9 @@
       <c r="CC337" t="n">
         <v>0</v>
       </c>
+      <c r="CD337" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="inlineStr">
@@ -75009,6 +76020,9 @@
       <c r="CC338" t="n">
         <v>1</v>
       </c>
+      <c r="CD338" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="inlineStr">
@@ -75230,6 +76244,9 @@
       <c r="CC339" t="n">
         <v>1</v>
       </c>
+      <c r="CD339" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="inlineStr">
@@ -75451,6 +76468,9 @@
       <c r="CC340" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD340" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="inlineStr">
@@ -75672,6 +76692,9 @@
       <c r="CC341" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD341" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="inlineStr">
@@ -75893,6 +76916,9 @@
       <c r="CC342" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD342" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" s="1" t="inlineStr">
@@ -76114,6 +77140,9 @@
       <c r="CC343" t="n">
         <v>0</v>
       </c>
+      <c r="CD343" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="inlineStr">
@@ -76335,6 +77364,9 @@
       <c r="CC344" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD344" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" s="1" t="inlineStr">
@@ -76556,6 +77588,9 @@
       <c r="CC345" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD345" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="inlineStr">
@@ -76777,6 +77812,9 @@
       <c r="CC346" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD346" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" s="1" t="inlineStr">
@@ -76998,6 +78036,9 @@
       <c r="CC347" t="n">
         <v>0</v>
       </c>
+      <c r="CD347" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="inlineStr">
@@ -77219,6 +78260,9 @@
       <c r="CC348" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD348" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="inlineStr">
@@ -77440,6 +78484,9 @@
       <c r="CC349" t="n">
         <v>0</v>
       </c>
+      <c r="CD349" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="inlineStr">
@@ -77661,6 +78708,9 @@
       <c r="CC350" t="n">
         <v>1</v>
       </c>
+      <c r="CD350" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" s="1" t="inlineStr">
@@ -77882,6 +78932,9 @@
       <c r="CC351" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD351" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" s="1" t="inlineStr">
@@ -78103,6 +79156,9 @@
       <c r="CC352" t="n">
         <v>0</v>
       </c>
+      <c r="CD352" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="inlineStr">
@@ -78324,6 +79380,9 @@
       <c r="CC353" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD353" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="inlineStr">
@@ -78545,6 +79604,9 @@
       <c r="CC354" t="n">
         <v>0.625</v>
       </c>
+      <c r="CD354" t="n">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="inlineStr">
@@ -78766,6 +79828,9 @@
       <c r="CC355" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD355" t="n">
+        <v>0.3333333333333333</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" s="1" t="inlineStr">
@@ -78987,6 +80052,9 @@
       <c r="CC356" t="n">
         <v>0</v>
       </c>
+      <c r="CD356" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" s="1" t="inlineStr">
@@ -79208,6 +80276,9 @@
       <c r="CC357" t="n">
         <v>0.6</v>
       </c>
+      <c r="CD357" t="n">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" s="1" t="inlineStr">
@@ -79429,6 +80500,9 @@
       <c r="CC358" t="n">
         <v>1</v>
       </c>
+      <c r="CD358" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" s="1" t="inlineStr">
@@ -79650,6 +80724,9 @@
       <c r="CC359" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD359" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" s="1" t="inlineStr">
@@ -79871,6 +80948,9 @@
       <c r="CC360" t="n">
         <v>0.4</v>
       </c>
+      <c r="CD360" t="n">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" s="1" t="inlineStr">
@@ -80092,6 +81172,9 @@
       <c r="CC361" t="n">
         <v>1</v>
       </c>
+      <c r="CD361" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" s="1" t="inlineStr">
@@ -80313,6 +81396,9 @@
       <c r="CC362" t="n">
         <v>1</v>
       </c>
+      <c r="CD362" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" s="1" t="inlineStr">
@@ -80534,6 +81620,9 @@
       <c r="CC363" t="n">
         <v>1</v>
       </c>
+      <c r="CD363" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" s="1" t="inlineStr">
@@ -80755,6 +81844,9 @@
       <c r="CC364" t="n">
         <v>0.1666666666666667</v>
       </c>
+      <c r="CD364" t="n">
+        <v>0.1666666666666667</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" s="1" t="inlineStr">
@@ -80976,6 +82068,9 @@
       <c r="CC365" t="n">
         <v>1</v>
       </c>
+      <c r="CD365" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" s="1" t="inlineStr">
@@ -81197,6 +82292,9 @@
       <c r="CC366" t="n">
         <v>0.625</v>
       </c>
+      <c r="CD366" t="n">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" s="1" t="inlineStr">
@@ -81418,6 +82516,9 @@
       <c r="CC367" t="n">
         <v>0.4</v>
       </c>
+      <c r="CD367" t="n">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" s="1" t="inlineStr">
@@ -81639,6 +82740,9 @@
       <c r="CC368" t="n">
         <v>1</v>
       </c>
+      <c r="CD368" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" s="1" t="inlineStr">
@@ -81860,6 +82964,9 @@
       <c r="CC369" t="n">
         <v>1</v>
       </c>
+      <c r="CD369" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" s="1" t="inlineStr">
@@ -82081,6 +83188,9 @@
       <c r="CC370" t="n">
         <v>0</v>
       </c>
+      <c r="CD370" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" s="1" t="inlineStr">
@@ -82302,6 +83412,9 @@
       <c r="CC371" t="n">
         <v>1</v>
       </c>
+      <c r="CD371" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" s="1" t="inlineStr">
@@ -82523,6 +83636,9 @@
       <c r="CC372" t="n">
         <v>1</v>
       </c>
+      <c r="CD372" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" s="1" t="inlineStr">
@@ -82744,6 +83860,9 @@
       <c r="CC373" t="n">
         <v>0</v>
       </c>
+      <c r="CD373" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" s="1" t="inlineStr">
@@ -82965,6 +84084,9 @@
       <c r="CC374" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD374" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" s="1" t="inlineStr">
@@ -83186,6 +84308,9 @@
       <c r="CC375" t="n">
         <v>1</v>
       </c>
+      <c r="CD375" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" s="1" t="inlineStr">
@@ -83407,6 +84532,9 @@
       <c r="CC376" t="n">
         <v>0</v>
       </c>
+      <c r="CD376" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" s="1" t="inlineStr">
@@ -83628,6 +84756,9 @@
       <c r="CC377" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD377" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" s="1" t="inlineStr">
@@ -83849,6 +84980,9 @@
       <c r="CC378" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD378" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" s="1" t="inlineStr">
@@ -84070,6 +85204,9 @@
       <c r="CC379" t="n">
         <v>1</v>
       </c>
+      <c r="CD379" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="380">
       <c r="A380" s="1" t="inlineStr">
@@ -84291,6 +85428,9 @@
       <c r="CC380" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD380" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="381">
       <c r="A381" s="1" t="inlineStr">
@@ -84512,6 +85652,9 @@
       <c r="CC381" t="n">
         <v>0.25</v>
       </c>
+      <c r="CD381" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="382">
       <c r="A382" s="1" t="inlineStr">
@@ -84733,6 +85876,9 @@
       <c r="CC382" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD382" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="383">
       <c r="A383" s="1" t="inlineStr">
@@ -84954,6 +86100,9 @@
       <c r="CC383" t="n">
         <v>0.1428571428571428</v>
       </c>
+      <c r="CD383" t="n">
+        <v>0.8571428571428571</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" s="1" t="inlineStr">
@@ -85175,6 +86324,9 @@
       <c r="CC384" t="n">
         <v>1</v>
       </c>
+      <c r="CD384" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="385">
       <c r="A385" s="1" t="inlineStr">
@@ -85396,6 +86548,9 @@
       <c r="CC385" t="n">
         <v>0</v>
       </c>
+      <c r="CD385" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="386">
       <c r="A386" s="1" t="inlineStr">
@@ -85617,6 +86772,9 @@
       <c r="CC386" t="n">
         <v>1</v>
       </c>
+      <c r="CD386" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="387">
       <c r="A387" s="1" t="inlineStr">
@@ -85838,6 +86996,9 @@
       <c r="CC387" t="n">
         <v>1</v>
       </c>
+      <c r="CD387" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="388">
       <c r="A388" s="1" t="inlineStr">
@@ -86059,6 +87220,9 @@
       <c r="CC388" t="n">
         <v>1</v>
       </c>
+      <c r="CD388" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="389">
       <c r="A389" s="1" t="inlineStr">
@@ -86280,6 +87444,9 @@
       <c r="CC389" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD389" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="390">
       <c r="A390" s="1" t="inlineStr">
@@ -86501,6 +87668,9 @@
       <c r="CC390" t="n">
         <v>0.5714285714285714</v>
       </c>
+      <c r="CD390" t="n">
+        <v>0.5714285714285714</v>
+      </c>
     </row>
     <row r="391">
       <c r="A391" s="1" t="inlineStr">
@@ -86722,6 +87892,9 @@
       <c r="CC391" t="n">
         <v>0</v>
       </c>
+      <c r="CD391" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="392">
       <c r="A392" s="1" t="inlineStr">
@@ -86943,6 +88116,9 @@
       <c r="CC392" t="n">
         <v>0.1818181818181818</v>
       </c>
+      <c r="CD392" t="n">
+        <v>0.8181818181818182</v>
+      </c>
     </row>
     <row r="393">
       <c r="A393" s="1" t="inlineStr">
@@ -87164,6 +88340,9 @@
       <c r="CC393" t="n">
         <v>1</v>
       </c>
+      <c r="CD393" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="394">
       <c r="A394" s="1" t="inlineStr">
@@ -87385,6 +88564,9 @@
       <c r="CC394" t="n">
         <v>1</v>
       </c>
+      <c r="CD394" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="395">
       <c r="A395" s="1" t="inlineStr">
@@ -87606,6 +88788,9 @@
       <c r="CC395" t="n">
         <v>1</v>
       </c>
+      <c r="CD395" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="396">
       <c r="A396" s="1" t="inlineStr">
@@ -87827,6 +89012,9 @@
       <c r="CC396" t="n">
         <v>1</v>
       </c>
+      <c r="CD396" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="397">
       <c r="A397" s="1" t="inlineStr">
@@ -88048,6 +89236,9 @@
       <c r="CC397" t="n">
         <v>1</v>
       </c>
+      <c r="CD397" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="398">
       <c r="A398" s="1" t="inlineStr">
@@ -88269,6 +89460,9 @@
       <c r="CC398" t="n">
         <v>1</v>
       </c>
+      <c r="CD398" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="399">
       <c r="A399" s="1" t="inlineStr">
@@ -88490,6 +89684,9 @@
       <c r="CC399" t="n">
         <v>0</v>
       </c>
+      <c r="CD399" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="400">
       <c r="A400" s="1" t="inlineStr">
@@ -88711,6 +89908,9 @@
       <c r="CC400" t="n">
         <v>0.75</v>
       </c>
+      <c r="CD400" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="401">
       <c r="A401" s="1" t="inlineStr">
@@ -88932,6 +90132,9 @@
       <c r="CC401" t="n">
         <v>0</v>
       </c>
+      <c r="CD401" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="402">
       <c r="A402" s="1" t="inlineStr">
@@ -89153,6 +90356,9 @@
       <c r="CC402" t="n">
         <v>0.5</v>
       </c>
+      <c r="CD402" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="403">
       <c r="A403" s="1" t="inlineStr">
@@ -89372,6 +90578,9 @@
         <v>1</v>
       </c>
       <c r="CC403" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD403" t="n">
         <v>1</v>
       </c>
     </row>
@@ -89471,6 +90680,7 @@
       <c r="CA404" t="inlineStr"/>
       <c r="CB404" t="inlineStr"/>
       <c r="CC404" t="inlineStr"/>
+      <c r="CD404" t="inlineStr"/>
     </row>
     <row r="405">
       <c r="A405" s="1" t="inlineStr">
@@ -89718,6 +90928,9 @@
       <c r="CC405" t="n">
         <v>829</v>
       </c>
+      <c r="CD405" t="n">
+        <v>1936</v>
+      </c>
     </row>
     <row r="406">
       <c r="A406" s="1" t="inlineStr">
@@ -89965,6 +91178,9 @@
       <c r="CC406" t="n">
         <v>2188</v>
       </c>
+      <c r="CD406" t="n">
+        <v>2188</v>
+      </c>
     </row>
     <row r="407">
       <c r="A407" s="1" t="inlineStr">
@@ -90212,6 +91428,9 @@
       <c r="CC407" t="n">
         <v>0.3789</v>
       </c>
+      <c r="CD407" t="n">
+        <v>0.8848</v>
+      </c>
     </row>
     <row r="408">
       <c r="A408" s="1" t="inlineStr">
@@ -90459,6 +91678,9 @@
       <c r="CC408" t="n">
         <v>1978</v>
       </c>
+      <c r="CD408" t="n">
+        <v>1978</v>
+      </c>
     </row>
     <row r="409">
       <c r="A409" s="1" t="inlineStr">
@@ -90706,6 +91928,9 @@
       <c r="CC409" t="n">
         <v>2188</v>
       </c>
+      <c r="CD409" t="n">
+        <v>2188</v>
+      </c>
     </row>
     <row r="410">
       <c r="A410" s="1" t="inlineStr">
@@ -90953,6 +92178,9 @@
       <c r="CC410" t="n">
         <v>0.904</v>
       </c>
+      <c r="CD410" t="n">
+        <v>0.904</v>
+      </c>
     </row>
     <row r="411">
       <c r="A411" s="1" t="inlineStr">
@@ -91178,6 +92406,9 @@
       <c r="CC411" t="n">
         <v>996</v>
       </c>
+      <c r="CD411" t="n">
+        <v>1475</v>
+      </c>
     </row>
     <row r="412">
       <c r="A412" s="1" t="inlineStr">
@@ -91425,6 +92656,9 @@
       <c r="CC412" t="n">
         <v>2188</v>
       </c>
+      <c r="CD412" t="n">
+        <v>2188</v>
+      </c>
     </row>
     <row r="413">
       <c r="A413" s="1" t="inlineStr">
@@ -91648,6 +92882,9 @@
       <c r="CC413" t="n">
         <v>0.4552</v>
       </c>
+      <c r="CD413" t="n">
+        <v>0.6741</v>
+      </c>
     </row>
     <row r="414">
       <c r="A414" s="1" t="inlineStr">
@@ -91895,6 +93132,9 @@
       <c r="CC414" t="n">
         <v>829</v>
       </c>
+      <c r="CD414" t="n">
+        <v>968</v>
+      </c>
     </row>
     <row r="415">
       <c r="A415" s="1" t="inlineStr">
@@ -92142,6 +93382,9 @@
       <c r="CC415" t="n">
         <v>2188</v>
       </c>
+      <c r="CD415" t="n">
+        <v>2188</v>
+      </c>
     </row>
     <row r="416">
       <c r="A416" s="1" t="inlineStr">
@@ -92389,6 +93632,9 @@
       <c r="CC416" t="n">
         <v>0.3789</v>
       </c>
+      <c r="CD416" t="n">
+        <v>0.4424</v>
+      </c>
     </row>
     <row r="417">
       <c r="A417" s="1" t="inlineStr">
@@ -92636,6 +93882,9 @@
       <c r="CC417" t="n">
         <v>2188</v>
       </c>
+      <c r="CD417" t="n">
+        <v>2188</v>
+      </c>
     </row>
     <row r="418">
       <c r="A418" s="1" t="inlineStr">
@@ -92883,6 +94132,9 @@
       <c r="CC418" t="n">
         <v>2188</v>
       </c>
+      <c r="CD418" t="n">
+        <v>2188</v>
+      </c>
     </row>
     <row r="419">
       <c r="A419" s="1" t="inlineStr">
@@ -93130,6 +94382,9 @@
       <c r="CC419" t="n">
         <v>1</v>
       </c>
+      <c r="CD419" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>